<commit_message>
fix tạo gg sheet
</commit_message>
<xml_diff>
--- a/src/public/samples/create-multiple-account.xlsx
+++ b/src/public/samples/create-multiple-account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\webbankhoahoc\backend\src\public\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8E3052-4AD4-4469-91AD-3F3F18D4028F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E0FBC9-6AC3-484B-8061-4EE8BFB79D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66EBCBF0-8B5F-4925-8347-3CFF073396F6}"/>
   </bookViews>
@@ -679,7 +679,7 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>